<commit_message>
Tab name is now imported as type, if type is not specified by user in either Excel or in meta parameters
</commit_message>
<xml_diff>
--- a/inst/extdata/james_example.xlsx
+++ b/inst/extdata/james_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C822CC-FEE6-3447-BED2-B24EB511C80F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6C784-4FC0-1A45-B3A3-9D0B6B3BEA44}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E6F58C3-28B5-A945-A3C1-97A0DEA814F4}"/>
+    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{9E6F58C3-28B5-A945-A3C1-97A0DEA814F4}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>tab</t>
   </si>
@@ -44,9 +44,6 @@
     <t>scenario</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
   <si>
     <t>title 1</t>
@@ -441,15 +435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3011D4F6-5D8F-6D4B-9131-8262A2331F56}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,42 +454,33 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -518,10 +501,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -753,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D99F1E0-F997-B84B-90FF-9760E7081C1C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -761,15 +744,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -780,7 +763,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>3</v>

</xml_diff>